<commit_message>
[CHG] INICIALIZANDO PÁGINA DE PLAN ESTRATEGICO
</commit_message>
<xml_diff>
--- a/src/data/FOOTPRINT_PLANEJAMENTO_ESTRATEGICO.xlsx
+++ b/src/data/FOOTPRINT_PLANEJAMENTO_ESTRATEGICO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson\Desktop\Analytics\MATERIAIS POR TEMA\STREAMLIT\APP_FOOTPRINT_PLANEJAMENTO_ESTRATEGICO\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson\Desktop\Analytics\MATERIAIS POR TEMA\STREAMLIT\APP_FOOTPRINT_PLANEJAMENTO_ESTRATEGICO\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>CÓDIGO AG</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t xml:space="preserve">         Receptora 20</t>
+  </si>
+  <si>
+    <t>REGIÃO</t>
+  </si>
+  <si>
+    <t>SUPT</t>
+  </si>
+  <si>
+    <t>DICOM</t>
   </si>
 </sst>
 </file>
@@ -356,7 +365,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -379,13 +388,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -692,15 +715,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,8 +767,17 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -790,8 +820,17 @@
       <c r="N2">
         <v>-46.770276600000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>13</v>
+      </c>
+      <c r="Q2">
+        <v>3</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -834,8 +873,17 @@
       <c r="N3">
         <v>-43.301957799999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -878,8 +926,17 @@
       <c r="N4">
         <v>-46.648072999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>18</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -922,8 +979,17 @@
       <c r="N5">
         <v>-47.4005279</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>19</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -967,8 +1033,17 @@
       <c r="N6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>12</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1011,8 +1086,17 @@
       <c r="N7">
         <v>-54.621886400000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>9</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1055,8 +1139,17 @@
       <c r="N8">
         <v>-43.182604900000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1099,8 +1192,17 @@
       <c r="N9">
         <v>-34.896998546294292</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1143,8 +1245,17 @@
       <c r="N10">
         <v>-34.882148880006042</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>14</v>
+      </c>
+      <c r="Q10">
+        <v>4</v>
+      </c>
+      <c r="R10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1187,8 +1298,17 @@
       <c r="N11">
         <v>-48.950681699999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>18</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1234,8 +1354,17 @@
       <c r="O12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>9</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1281,8 +1410,17 @@
       <c r="O13" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1328,8 +1466,17 @@
       <c r="O14" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1375,8 +1522,17 @@
       <c r="O15" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1422,8 +1578,17 @@
       <c r="O16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>14</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1469,8 +1634,17 @@
       <c r="O17" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>3</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1516,8 +1690,17 @@
       <c r="O18" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1563,8 +1746,17 @@
       <c r="O19" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>13</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1610,8 +1802,17 @@
       <c r="O20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>17</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1656,6 +1857,15 @@
       </c>
       <c r="O21" t="s">
         <v>101</v>
+      </c>
+      <c r="P21">
+        <v>7</v>
+      </c>
+      <c r="Q21">
+        <v>4</v>
+      </c>
+      <c r="R21">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>